<commit_message>
Teste de unificação de lista de presença
</commit_message>
<xml_diff>
--- a/presenca.xlsx
+++ b/presenca.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/561e3191c080ffc5/Documentos/dev/coletivoAprendiz/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\JOBS\Cieds\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{AA36A75E-37E9-4BC5-86CB-EEB90BCB1630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B64A1922-6885-4202-8248-BF1F7EC40F35}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D31EA6F6-189F-4929-83D0-E7ED03D4D7B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{AADD3DBC-10A2-4E1E-B84E-2ACBCC221757}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AADD3DBC-10A2-4E1E-B84E-2ACBCC221757}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t>Página 1</t>
   </si>
@@ -184,6 +184,42 @@
   <si>
     <t>COMPANHIA DOCAS DO RIO DE JANEIRO</t>
   </si>
+  <si>
+    <t>Joao Marcos</t>
+  </si>
+  <si>
+    <t>Priscila Monteiro</t>
+  </si>
+  <si>
+    <t>Otavio Henrique</t>
+  </si>
+  <si>
+    <t>Gabriel Fernando</t>
+  </si>
+  <si>
+    <t>Andre Muller</t>
+  </si>
+  <si>
+    <t>Antonio conselheiro</t>
+  </si>
+  <si>
+    <t>Pantera negra</t>
+  </si>
+  <si>
+    <t>Chico Science</t>
+  </si>
+  <si>
+    <t>Tomé de Souza</t>
+  </si>
+  <si>
+    <t>Padre anchieta</t>
+  </si>
+  <si>
+    <t>Antonio Bandeirante</t>
+  </si>
+  <si>
+    <t>José Prudente de Morais</t>
+  </si>
 </sst>
 </file>
 
@@ -192,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-10409]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -237,20 +273,6 @@
       <color rgb="FF4D4D4D"/>
       <name val="Tahoma"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="7.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -330,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -339,30 +361,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -379,6 +377,36 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -388,20 +416,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,9 +829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C4A81B-6DDE-4A06-A129-9EA8C6FFFC9B}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15:C15"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,137 +861,137 @@
   <sheetData>
     <row r="1" spans="1:20" ht="3.4" customHeight="1"/>
     <row r="2" spans="1:20">
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="13"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:20" ht="16.350000000000001" customHeight="1">
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:20" ht="41.45" customHeight="1">
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1">
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="5.0999999999999996" customHeight="1"/>
     <row r="7" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="2.1" customHeight="1"/>
     <row r="9" spans="1:20">
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="J10" s="17">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="9">
         <v>45154</v>
       </c>
-      <c r="K10" s="13"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:20" ht="9.9499999999999993" customHeight="1"/>
     <row r="13" spans="1:20" ht="3.95" customHeight="1"/>
     <row r="14" spans="1:20" ht="17.100000000000001" customHeight="1">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="6"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="12"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="12"/>
+      <c r="D15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="10" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="11" t="s">
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="11" t="s">
+      <c r="L15" s="12"/>
+      <c r="M15" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="11" t="s">
+      <c r="N15" s="11"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="6"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="2" t="s">
         <v>11</v>
       </c>
@@ -984,33 +1000,35 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="B16" s="4">
+      <c r="B16" s="19">
         <v>52967</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="7" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="6"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1019,33 +1037,35 @@
       </c>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="4">
+      <c r="B17" s="19">
         <v>51762</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="7" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="6"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="12"/>
+      <c r="M17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="11"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="12"/>
       <c r="S17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1054,33 +1074,35 @@
       </c>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="4">
+      <c r="B18" s="19">
         <v>59259</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="7" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="6"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="11"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1089,33 +1111,35 @@
       </c>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="4">
+      <c r="B19" s="19">
         <v>38819</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="7" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="6"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="11"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1124,33 +1148,35 @@
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="4">
+      <c r="B20" s="19">
         <v>59690</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="7" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="6"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="11"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="12"/>
       <c r="S20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1159,43 +1185,49 @@
       </c>
     </row>
     <row r="21" spans="2:20" ht="17.100000000000001" customHeight="1">
-      <c r="B21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="6"/>
+      <c r="B21" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="O2:P3"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="E5:M5"/>
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="F9:H11"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B14:T14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="B21:T21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:G16"/>
@@ -1208,25 +1240,19 @@
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="B21:T21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="B14:T14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="O2:P3"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="E5:M5"/>
+    <mergeCell ref="A7:Q7"/>
+    <mergeCell ref="F9:H11"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="1.30782283464567" header="0.59055118110236204" footer="0.78740157480314998"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1241,9 +1267,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3637E5C4-A4FF-4100-926D-0B70C0524C25}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21:J21"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1273,136 +1299,136 @@
   <sheetData>
     <row r="1" spans="1:20" ht="3.4" customHeight="1"/>
     <row r="2" spans="1:20">
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="13"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:20" ht="16.350000000000001" customHeight="1">
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:20" ht="41.45" customHeight="1">
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:20" ht="17.100000000000001" customHeight="1">
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="5.0999999999999996" customHeight="1"/>
     <row r="7" spans="1:20" ht="24.95" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="2.1" customHeight="1"/>
     <row r="9" spans="1:20">
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="J10" s="17">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="9">
         <v>45154</v>
       </c>
-      <c r="K10" s="13"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:20" ht="9.9499999999999993" customHeight="1"/>
     <row r="13" spans="1:20" ht="17.100000000000001" customHeight="1">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="6"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="10" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="11" t="s">
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="11" t="s">
+      <c r="L14" s="12"/>
+      <c r="M14" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="11" t="s">
+      <c r="N14" s="11"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="6"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="12"/>
       <c r="S14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1411,33 +1437,35 @@
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="B15" s="4">
+      <c r="B15" s="19">
         <v>43865</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7" t="s">
+      <c r="C15" s="12"/>
+      <c r="D15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="6"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="12"/>
       <c r="S15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1446,33 +1474,35 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="B16" s="4">
+      <c r="B16" s="19">
         <v>47933</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="6"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="12"/>
       <c r="S16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1481,33 +1511,35 @@
       </c>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="4">
+      <c r="B17" s="19">
         <v>45521</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="6"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="12"/>
+      <c r="M17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="11"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="12"/>
       <c r="S17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1516,33 +1548,35 @@
       </c>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="4">
+      <c r="B18" s="19">
         <v>47919</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="6"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="11"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="12"/>
       <c r="S18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1551,33 +1585,35 @@
       </c>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="4">
+      <c r="B19" s="19">
         <v>47767</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="7" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="6"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="11"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="12"/>
       <c r="S19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1586,33 +1622,35 @@
       </c>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="4">
+      <c r="B20" s="19">
         <v>48010</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="6"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" s="11"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="12"/>
       <c r="S20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1621,33 +1659,35 @@
       </c>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="4">
+      <c r="B21" s="19">
         <v>39103</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="6"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="11"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="12"/>
       <c r="S21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1656,43 +1696,61 @@
       </c>
     </row>
     <row r="22" spans="2:20" ht="17.100000000000001" customHeight="1">
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="6"/>
+      <c r="B22" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="O2:P3"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="E5:M5"/>
-    <mergeCell ref="A7:Q7"/>
-    <mergeCell ref="F9:H11"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B13:T13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="B22:T22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:O18"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:G15"/>
@@ -1705,37 +1763,19 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="B22:T22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="B13:T13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="O2:P3"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="E5:M5"/>
+    <mergeCell ref="A7:Q7"/>
+    <mergeCell ref="F9:H11"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="1.30782283464567" header="0.59055118110236204" footer="0.78740157480314998"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>